<commit_message>
Adding GLIDE number impact estimates and continuing to adapt the GCDB_tab object structure
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/GLIDE-HIP.xlsx
+++ b/Taxonomies/MostlyImpactData/GLIDE-HIP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t xml:space="preserve">haz_Ab</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">haz_spec</t>
   </si>
   <si>
+    <t xml:space="preserve">haz_potlink</t>
+  </si>
+  <si>
     <t xml:space="preserve">AC</t>
   </si>
   <si>
@@ -106,25 +109,7 @@
     <t xml:space="preserve">ET</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0047,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0040,MH0042,MH0043,MH0037,MH0038,MH0039</t>
-    </r>
+    <t xml:space="preserve">MH0047,MH0040,MH0042,MH0043,MH0037,MH0038,MH0039</t>
   </si>
   <si>
     <t xml:space="preserve">FA</t>
@@ -148,67 +133,13 @@
     <t xml:space="preserve">FR</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">haztypeenviron,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">haztypetech</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">hazenvenvdeg,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">haztechindfail</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">EN0013,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">TL0032</t>
-    </r>
+    <t xml:space="preserve">haztypeenviron,haztypetech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hazenvenvdeg,haztechindfail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN0013,TL0032</t>
   </si>
   <si>
     <t xml:space="preserve">HT</t>
@@ -223,25 +154,7 @@
     <t xml:space="preserve">hazbioinfest</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BI0002,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">BI0003</t>
-    </r>
+    <t xml:space="preserve">BI0002,BI0003</t>
   </si>
   <si>
     <t xml:space="preserve">LS</t>
@@ -426,7 +339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -467,12 +380,6 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -545,7 +452,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,7 +476,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -591,364 +498,366 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>